<commit_message>
Updated scraper for more robust and consistent data pull
</commit_message>
<xml_diff>
--- a/starving_student.xlsx
+++ b/starving_student.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srobi\Projects\Starving_Student\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D04D3E2-5AF6-4676-8DCA-9E3593F62886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56C9996-E462-4ADE-9436-901FA817E450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{560CFB3B-6B42-4BA3-BC39-FDF24F6D64B4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{560CFB3B-6B42-4BA3-BC39-FDF24F6D64B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="91">
   <si>
     <t>User inputs</t>
   </si>
@@ -264,9 +264,6 @@
     <t>uom</t>
   </si>
   <si>
-    <t>grams</t>
-  </si>
-  <si>
     <t>salad</t>
   </si>
   <si>
@@ -301,6 +298,15 @@
   </si>
   <si>
     <t>https://www.feastingathome.com/quick-chickpea-biryani/</t>
+  </si>
+  <si>
+    <t>ounce</t>
+  </si>
+  <si>
+    <t>gram</t>
+  </si>
+  <si>
+    <t>cup</t>
   </si>
 </sst>
 </file>
@@ -719,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378DAD80-777F-48AD-8169-32D9FFA89C07}">
   <dimension ref="B2:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,7 +762,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>48</v>
@@ -826,7 +832,7 @@
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>49</v>
@@ -858,13 +864,13 @@
         <v>60</v>
       </c>
       <c r="E20" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="G20" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>30</v>
@@ -905,7 +911,7 @@
         <v>33</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E21" s="1">
         <v>5</v>
@@ -914,7 +920,7 @@
         <v>60</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>34</v>
@@ -949,13 +955,13 @@
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E22" s="1">
         <v>6</v>
@@ -964,7 +970,7 @@
         <v>45</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>34</v>
@@ -994,7 +1000,7 @@
         <v>36</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.25">
@@ -1026,7 +1032,7 @@
         <v>37</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.25">
@@ -1046,7 +1052,7 @@
         <v>57</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R24" s="1" t="s">
         <v>5</v>
@@ -1078,7 +1084,7 @@
         <v>58</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R25" s="1" t="s">
         <v>11</v>
@@ -1090,7 +1096,7 @@
         <v>39</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.25">

</xml_diff>